<commit_message>
OUCD legend, oecd xml function points
</commit_message>
<xml_diff>
--- a/SoftwareEngeneering/Function Point Calculation.xlsx
+++ b/SoftwareEngeneering/Function Point Calculation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpenkert/Development/AlarmClock/SimpleHabits/SoftwareEngeneering/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bene/Documents/Programmieren/SimpleHabits/SoftwareEngeneering/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -327,7 +327,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Function point</a:t>
+              <a:t>Function points</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -398,7 +398,7 @@
                 </a:gsLst>
                 <a:lin ang="5400000" scaled="0"/>
               </a:gradFill>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="63500" cap="flat" cmpd="sng" algn="ctr">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:shade val="95000"/>
@@ -411,51 +411,24 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$L$3:$L$9</c:f>
+              <c:f>Tabelle1!$L$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>20.15</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.05</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>33.6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>61.60000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>114.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$I$3:$I$6</c:f>
+              <c:f>Tabelle1!$I$3</c:f>
               <c:numCache>
                 <c:formatCode>h:mm</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>0.458333333333333</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.420138888888889</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.277777777777778</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.878472222222222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -467,6 +440,156 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Determine Home location</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln w="63500"/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>13.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.420138888888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enter offset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln w="63500"/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.277777777777778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRUD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln w="63500"/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$L$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>33.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.878472222222222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -475,11 +598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="881025584"/>
-        <c:axId val="881027632"/>
+        <c:axId val="-1695424976"/>
+        <c:axId val="-1695108848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="881025584"/>
+        <c:axId val="-1695424976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,12 +659,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881027632"/>
+        <c:crossAx val="-1695108848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="881027632"/>
+        <c:axId val="-1695108848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +721,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="881025584"/>
+        <c:crossAx val="-1695424976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -624,6 +747,11 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -669,20 +797,20 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>15875</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>187324</xdr:rowOff>
+      <xdr:rowOff>187323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>31749</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>173674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Diagramm 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -707,19 +835,19 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.08088</cdr:x>
-      <cdr:y>0.17915</cdr:y>
+      <cdr:x>0.07653</cdr:x>
+      <cdr:y>0.16999</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.88624</cdr:x>
-      <cdr:y>0.92978</cdr:y>
+      <cdr:x>0.87774</cdr:x>
+      <cdr:y>0.78727</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
         <cdr:cNvPr id="10" name="Gerader Verbinder 9">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66E24313-CBBA-42E7-8025-CC9B0A7AD064}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66E24313-CBBA-42E7-8025-CC9B0A7AD064}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -727,12 +855,13 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="602670" y="472508"/>
-          <a:ext cx="6001064" cy="1979742"/>
+          <a:off x="570279" y="529087"/>
+          <a:ext cx="5970085" cy="1921283"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="6350"/>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
@@ -849,8 +978,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabelle15" displayName="Tabelle15" ref="O16:Q17" totalsRowShown="0">
-  <autoFilter ref="O16:Q17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabelle15" displayName="Tabelle15" ref="O19:Q20" totalsRowShown="0">
+  <autoFilter ref="O19:Q20"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Time spent (w/o outliers)" dataDxfId="3">
       <calculatedColumnFormula>SUM(I3:I6)*24</calculatedColumnFormula>
@@ -859,7 +988,7 @@
       <calculatedColumnFormula>SUM(L3:L6)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Velocity" dataDxfId="2">
-      <calculatedColumnFormula>P17/O17</calculatedColumnFormula>
+      <calculatedColumnFormula>P20/O20</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1216,8 +1345,8 @@
   <sheetPr codeName="Tabelle1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B2:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="117" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="117" zoomScaleNormal="117" zoomScalePageLayoutView="117" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1230,7 +1359,7 @@
     <col min="15" max="15" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1397,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>34</v>
       </c>
@@ -1307,7 +1436,7 @@
         <v>20.150000000000002</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -1346,7 +1475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1385,7 +1514,7 @@
         <v>11.05</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>38</v>
       </c>
@@ -1424,7 +1553,7 @@
         <v>33.6</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1464,7 +1593,7 @@
       </c>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>40</v>
       </c>
@@ -1503,7 +1632,7 @@
         <v>28.000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>41</v>
       </c>
@@ -1542,7 +1671,7 @@
         <v>114.80000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1553,7 +1682,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -1585,7 +1714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +1748,7 @@
         <v>20.150000000000002</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>20</v>
       </c>
@@ -1649,7 +1778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>21</v>
       </c>
@@ -1679,7 +1808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>22</v>
       </c>
@@ -1708,15 +1837,6 @@
         <f>Tabelle2[[#This Row],[Count]]*(7*Tabelle2[[#This Row],[Simple]]+10*Tabelle2[[#This Row],[Average]]+15*Tabelle2[[#This Row],[Complex]])</f>
         <v>21</v>
       </c>
-      <c r="O16" t="s">
-        <v>23</v>
-      </c>
-      <c r="P16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
@@ -1747,17 +1867,16 @@
         <f>Tabelle2[[#This Row],[Count]]*(5*Tabelle2[[#This Row],[Simple]]+7*Tabelle2[[#This Row],[Average]]+10*Tabelle2[[#This Row],[Complex]])</f>
         <v>0</v>
       </c>
-      <c r="O17" s="4">
-        <f>SUM(I3:I6)*24</f>
-        <v>48.833333333333336</v>
-      </c>
-      <c r="P17">
-        <f>SUM(L3:L6)</f>
-        <v>77.800000000000011</v>
-      </c>
-      <c r="Q17" s="3">
-        <f>P17/O17</f>
-        <v>1.5931740614334473</v>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="O19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
@@ -1790,6 +1909,18 @@
       </c>
       <c r="K20" t="s">
         <v>18</v>
+      </c>
+      <c r="O20" s="4">
+        <f>SUM(I3:I6)*24</f>
+        <v>48.833333333333336</v>
+      </c>
+      <c r="P20">
+        <f>SUM(L3:L6)</f>
+        <v>77.800000000000011</v>
+      </c>
+      <c r="Q20" s="3">
+        <f>P20/O20</f>
+        <v>1.5931740614334473</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>